<commit_message>
Updated tasks file and added tasks for week 2
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="35">
   <si>
     <t>Develop endpoint for Arduino</t>
   </si>
@@ -85,13 +85,52 @@
   </si>
   <si>
     <t>Me</t>
+  </si>
+  <si>
+    <t>6 hours</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>12.4.2017</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>12.5.2017</t>
+  </si>
+  <si>
+    <t>0 hours</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>12.6.2017</t>
+  </si>
+  <si>
+    <t>Василен</t>
+  </si>
+  <si>
+    <t>12.10.2017</t>
+  </si>
+  <si>
+    <t>Refactor server database architecture</t>
+  </si>
+  <si>
+    <t>Research for popular android libraries and controllers</t>
+  </si>
+  <si>
+    <t>11.10.2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,8 +145,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +170,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -129,16 +192,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,207 +530,383 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="1">
-        <v>1</v>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>